<commit_message>
- Added faker library - Fixed test
</commit_message>
<xml_diff>
--- a/src/test/resources/ExecutionFlow.xlsx
+++ b/src/test/resources/ExecutionFlow.xlsx
@@ -32,12 +32,12 @@
     <t>ID</t>
   </si>
   <si>
+    <t>scenario</t>
+  </si>
+  <si>
     <t>class name</t>
   </si>
   <si>
-    <t>scenario</t>
-  </si>
-  <si>
     <t>Method name</t>
   </si>
   <si>
@@ -47,10 +47,10 @@
     <t>001</t>
   </si>
   <si>
+    <t>webInputsTest</t>
+  </si>
+  <si>
     <t>ExpandTests</t>
-  </si>
-  <si>
-    <t>webInputsTest</t>
   </si>
   <si>
     <t>002</t>
@@ -810,6 +810,22 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1080,14 +1096,15 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="4.57142857142857" customWidth="1"/>
-    <col min="2" max="2" width="12.8571428571429" customWidth="1"/>
-    <col min="3" max="4" width="25" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="12.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="6.71428571428571" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1119,10 +1136,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1130,16 +1147,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1147,16 +1164,16 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1164,16 +1181,16 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1181,16 +1198,16 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1198,16 +1215,16 @@
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1215,10 +1232,10 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>19</v>
@@ -1232,16 +1249,16 @@
         <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1249,10 +1266,10 @@
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>23</v>
@@ -1266,16 +1283,16 @@
         <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1283,16 +1300,16 @@
         <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1300,16 +1317,16 @@
         <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1317,16 +1334,16 @@
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1334,16 +1351,16 @@
         <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1351,16 +1368,16 @@
         <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1368,19 +1385,42 @@
         <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E17" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:E1048576">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8 E2:E7 E9:E1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
-Removed duplicate dependency - Fixed static problem
</commit_message>
<xml_diff>
--- a/src/test/resources/ExecutionFlow.xlsx
+++ b/src/test/resources/ExecutionFlow.xlsx
@@ -1096,7 +1096,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1139,7 +1139,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1156,7 +1156,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1173,7 +1173,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1190,7 +1190,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1207,7 +1207,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1224,7 +1224,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1258,7 +1258,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1275,7 +1275,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1292,7 +1292,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1309,7 +1309,7 @@
         <v>27</v>
       </c>
       <c r="E12" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1326,7 +1326,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1343,7 +1343,7 @@
         <v>31</v>
       </c>
       <c r="E14" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1360,7 +1360,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1377,7 +1377,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1394,7 +1394,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1417,7 +1417,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8 E2:E7 E9:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added test automation play ground tests
</commit_message>
<xml_diff>
--- a/src/test/resources/ExecutionFlow.xlsx
+++ b/src/test/resources/ExecutionFlow.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -141,6 +141,57 @@
   </si>
   <si>
     <t>scrollBar</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>waitActionsTest</t>
+  </si>
+  <si>
+    <t>AutomationPlaygroundTests</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>popUpWindowsTest</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>framesTest</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>mouseActionsTest</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>keyboardActions</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>formPageTests</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>samplePageTest</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>advancedUITests</t>
   </si>
 </sst>
 </file>
@@ -1093,17 +1144,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="4.57142857142857" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="12.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="36.7142857142857" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="6.71428571428571" customWidth="1"/>
   </cols>
@@ -1241,7 +1292,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1394,6 +1445,139 @@
         <v>37</v>
       </c>
       <c r="E17" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new methods to sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/ExecutionFlow.xlsx
+++ b/src/test/resources/ExecutionFlow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24000" windowHeight="9480"/>
+    <workbookView windowWidth="24000" windowHeight="8760"/>
   </bookViews>
   <sheets>
     <sheet name="control" sheetId="2" r:id="rId1"/>
@@ -1147,7 +1147,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -1460,6 +1460,9 @@
       </c>
       <c r="D18" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1527,7 +1530,7 @@
         <v>48</v>
       </c>
       <c r="E22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1544,7 +1547,7 @@
         <v>50</v>
       </c>
       <c r="E23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1561,7 +1564,7 @@
         <v>52</v>
       </c>
       <c r="E24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1578,7 +1581,7 @@
         <v>54</v>
       </c>
       <c r="E25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1601,7 +1604,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E17 E18:E25 E26:E1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added maven surefire plugin
</commit_message>
<xml_diff>
--- a/src/test/resources/ExecutionFlow.xlsx
+++ b/src/test/resources/ExecutionFlow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24000" windowHeight="8760"/>
+    <workbookView windowWidth="24000" windowHeight="9480"/>
   </bookViews>
   <sheets>
     <sheet name="control" sheetId="2" r:id="rId1"/>
@@ -1147,7 +1147,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1462,7 +1462,7 @@
         <v>39</v>
       </c>
       <c r="E18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1513,7 +1513,7 @@
         <v>46</v>
       </c>
       <c r="E21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1530,7 +1530,7 @@
         <v>48</v>
       </c>
       <c r="E22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1547,7 +1547,7 @@
         <v>50</v>
       </c>
       <c r="E23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1564,7 +1564,7 @@
         <v>52</v>
       </c>
       <c r="E24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1581,7 +1581,7 @@
         <v>54</v>
       </c>
       <c r="E25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1604,7 +1604,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E17 E18:E25 E26:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E21 E22 E23 E24 E25 E2:E20 E26:E1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fixed new tab wait problem
</commit_message>
<xml_diff>
--- a/src/test/resources/ExecutionFlow.xlsx
+++ b/src/test/resources/ExecutionFlow.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>003</t>
+  </si>
+  <si>
+    <t>Register test</t>
+  </si>
+  <si>
+    <t>registertest</t>
   </si>
   <si>
     <t>otpTest</t>
@@ -1144,10 +1150,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1221,7 +1227,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -1229,7 +1235,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -1456,7 +1462,7 @@
         <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>39</v>
@@ -1467,16 +1473,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" t="b">
         <v>1</v>
@@ -1490,7 +1496,7 @@
         <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>44</v>
@@ -1507,7 +1513,7 @@
         <v>46</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>46</v>
@@ -1524,7 +1530,7 @@
         <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>48</v>
@@ -1541,7 +1547,7 @@
         <v>50</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>50</v>
@@ -1558,7 +1564,7 @@
         <v>52</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>52</v>
@@ -1575,12 +1581,29 @@
         <v>54</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1604,7 +1627,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E25 E26:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E2:E3 E5:E1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Enabled all automation playground tests
</commit_message>
<xml_diff>
--- a/src/test/resources/ExecutionFlow.xlsx
+++ b/src/test/resources/ExecutionFlow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24000" windowHeight="8760"/>
+    <workbookView windowWidth="24000" windowHeight="9480"/>
   </bookViews>
   <sheets>
     <sheet name="control" sheetId="2" r:id="rId1"/>
@@ -1153,7 +1153,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1604,7 +1604,7 @@
         <v>56</v>
       </c>
       <c r="E26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1627,7 +1627,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26 E2:E25 E27:E1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>